<commit_message>
web: update markets add profit factor
</commit_message>
<xml_diff>
--- a/docs/reports/markets_2015-2025.xlsx
+++ b/docs/reports/markets_2015-2025.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="US stocks (S&amp;P500)" sheetId="1" state="visible" r:id="rId3"/>
@@ -199,7 +199,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="254">
   <si>
     <t xml:space="preserve">Ticker</t>
   </si>
@@ -411,217 +411,220 @@
     <t xml:space="preserve">Consumer Goods (Luxury Goods)</t>
   </si>
   <si>
-    <t xml:space="preserve">NSE:POWERGRID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Power Grid Corporation of India Limited</t>
+    <t xml:space="preserve">NSE:BAJAJFINSV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bajaj Finserv Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finance (Insurance)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSE:ADANIENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adani Enterprises Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Industrials (Conglomerate)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSE:TRENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trent Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSE:ZOMATO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zomato Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consumer Services (Food Delivery)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSE:VBL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Varun Beverages Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consumer Goods (Beverages)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSE:LTIM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Larsen &amp; Toubro Infotech Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSE:ADANIPOWER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adani Power Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilities (Power Generation)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSE:IOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indian Oil Corporation Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy (Oil &amp; Gas)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSE:IRFC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indian Railway Finance Corporation Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finance (Infrastructure Finance)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSE:TATASTEEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tata Steel Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Materials (Steel Production)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSE:SBILIFE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBILife Insurance Company Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSE:ADANIGREEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adani Green Energy Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilities (Renewable Energy)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSE:BRITANNIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Britannia Industries Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSE:RECLTD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rural Electrification Corporation Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSE:BAJAJHLDNG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bajaj Holdings &amp; Investment Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finance (Investment)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSE:TVSMOTOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TVS Motor Company LTD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consumer Durables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BCBA:YPFD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YPF S.A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BCBA:GGAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grupo Galicia S.A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BCBA:TECO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tecpetrol S.A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BCBA:PAMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pampa Energía S.A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy (Electricity &amp; Gas)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BCBA:VIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vistage International</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BCBA:TGSU2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transportadora de Gas del Sur S.A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilities (Natural Gas Transmission)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BCBA:TXAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transportadora de Gas del Norte S.A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BCBA:CEPU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central Puerto S.A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy (Electricity Generation)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BCBA:BPAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Banco Patagonia S.A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BCBA:SUPV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supervielle S.A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BCBA:BYMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bolsas y Mercados Argentinos S.A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finance (Stock Exchange)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BCBA:EDN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empresa Distribuidora y Comercializadora Norte S.A.</t>
   </si>
   <si>
     <t xml:space="preserve">Utilities (Electricity Distribution)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NSE:BAJAJFINSV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bajaj Finserv Limited</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finance (Insurance)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NSE:ADANIENT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adani Enterprises Limited</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Industrials (Conglomerate)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NSE:TRENT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trent Limited</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NSE:ZOMATO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zomato Limited</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consumer Services (Food Delivery)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NSE:VBL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Varun Beverages Limited</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consumer Goods (Beverages)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NSE:LTIM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Larsen &amp; Toubro Infotech Limited</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NSE:ADANIPOWER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adani Power Limited</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utilities (Power Generation)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NSE:IOC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indian Oil Corporation Limited</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Energy (Oil &amp; Gas)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NSE:IRFC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indian Railway Finance Corporation Limited</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finance (Infrastructure Finance)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NSE:TATASTEEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tata Steel Limited</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Materials (Steel Production)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NSE:SBILIFE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SBILife Insurance Company Limited</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NSE:ADANIGREEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adani Green Energy Limited</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utilities (Renewable Energy)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NSE:BRITANNIA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Britannia Industries Limited</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NSE:RECLTD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rural Electrification Corporation Limited</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NSE:BAJAJHLDNG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bajaj Holdings &amp; Investment Limited</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finance (Investment)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BCBA:YPFD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YPF S.A.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BCBA:GGAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grupo Galicia S.A.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BCBA:TECO2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tecpetrol S.A.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BCBA:PAMP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pampa Energía S.A.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Energy (Electricity &amp; Gas)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BCBA:VIST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vistage International</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BCBA:TGSU2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transportadora de Gas del Sur S.A.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utilities (Natural Gas Transmission)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BCBA:TXAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transportadora de Gas del Norte S.A.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BCBA:CEPU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Central Puerto S.A.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Energy (Electricity Generation)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BCBA:BPAT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Banco Patagonia S.A.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BCBA:SUPV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supervielle S.A.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BCBA:BYMA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bolsas y Mercados Argentinos S.A.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finance (Stock Exchange)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BCBA:EDN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Empresa Distribuidora y Comercializadora Norte S.A.</t>
   </si>
   <si>
     <t xml:space="preserve">BCBA:LOMA</t>
@@ -968,11 +971,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -991,6 +995,12 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1038,16 +1048,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1176,320 +1190,320 @@
   </sheetPr>
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="26.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="29.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="33.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="26.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="29.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>3.239</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>3.289</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>2.352</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>2.288</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>2.145</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>2.543</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>2.11</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>2.424</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>4.415</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>2.86</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="1" t="n">
         <v>2.508</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <v>2.435</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="1" t="n">
         <v>2.387</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <v>3.699</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="1" t="n">
         <v>2.175</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="1" t="n">
         <v>2.354</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="1" t="n">
         <v>2.185</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="1" t="n">
         <v>2.61</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D20" s="1" t="n">
         <v>2.94</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21" s="1" t="n">
         <v>2.027</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D22" s="2" t="n">
+      <c r="D22" s="3" t="n">
         <f aca="false">AVERAGE(D2:D21)</f>
         <v>2.64925</v>
       </c>
@@ -1514,258 +1528,318 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="31.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>60</v>
       </c>
+      <c r="D2" s="1" t="n">
+        <v>2.133</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="D3" s="1" t="n">
+        <v>2.496</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="D4" s="1" t="n">
+        <v>2.347</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="D5" s="1" t="n">
+        <v>2.32</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>72</v>
       </c>
+      <c r="D6" s="0" t="n">
+        <v>4.078</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>75</v>
       </c>
+      <c r="D7" s="1" t="n">
+        <v>2.441</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>4.123</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>28</v>
+      <c r="D9" s="1" t="n">
+        <v>2.998</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>83</v>
       </c>
+      <c r="D10" s="1" t="n">
+        <v>2.324</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>3.548</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C12" s="0" t="s">
-        <v>60</v>
+      <c r="D12" s="1" t="n">
+        <v>2.517</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="D13" s="1" t="n">
+        <v>2.031</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="1" t="s">
         <v>94</v>
       </c>
+      <c r="D14" s="0" t="n">
+        <v>5.702</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="1" t="s">
         <v>97</v>
       </c>
+      <c r="D15" s="1" t="n">
+        <v>2.101</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>2.257</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="C17" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C17" s="0" t="s">
-        <v>75</v>
+      <c r="D17" s="0" t="n">
+        <v>3.15</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>2.934</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="C19" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>2.088</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C19" s="0" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="C20" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C20" s="0" t="s">
-        <v>97</v>
+      <c r="D20" s="1" t="n">
+        <v>2.41</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="1" t="s">
         <v>112</v>
       </c>
+      <c r="D21" s="1" t="n">
+        <v>2.995</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D22" s="0" t="e">
-        <f aca="false">AVERAGE(D2:D21)</f>
-        <v>#DIV/0!</v>
+      <c r="D22" s="1" t="n">
+        <f aca="false">AVERAGE(D2:D20)</f>
+        <v>2.842</v>
       </c>
     </row>
   </sheetData>
@@ -1788,258 +1862,318 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>94</v>
+      <c r="C2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>2.471</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="D3" s="1" t="n">
+        <v>3.715</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>94</v>
+      <c r="C4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>2.967</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>121</v>
       </c>
+      <c r="D5" s="1" t="n">
+        <v>4.978</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="D6" s="1" t="n">
+        <v>4.122</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>126</v>
       </c>
+      <c r="D7" s="1" t="n">
+        <v>3.884</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>126</v>
       </c>
+      <c r="D8" s="1" t="n">
+        <v>2.453</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>131</v>
       </c>
+      <c r="D9" s="1" t="n">
+        <v>5.708</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="D10" s="1" t="n">
+        <v>4.192</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="D11" s="1" t="n">
+        <v>5.049</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>138</v>
       </c>
+      <c r="D12" s="1" t="n">
+        <v>4.502</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C13" s="0" t="s">
-        <v>72</v>
+      <c r="C13" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>6.072</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="B14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="C14" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>2.746</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="B15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>146</v>
       </c>
+      <c r="C15" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>6.64</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>5.182</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>5.689</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B16" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="D18" s="1" t="n">
+        <v>3.143</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>4.694</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>8.922</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B18" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>152</v>
+      <c r="D21" s="1" t="n">
+        <v>2.3</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D22" s="0" t="e">
+      <c r="D22" s="1" t="n">
         <f aca="false">AVERAGE(D2:D21)</f>
-        <v>#DIV/0!</v>
+        <v>4.47145</v>
       </c>
     </row>
   </sheetData>
@@ -2062,258 +2196,318 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>161</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>3.883</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>164</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>3.614</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>2.096</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>4.152</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="D6" s="1" t="n">
+        <v>6.319</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>6.357</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>4.244</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>5.672</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>3.628</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>4.949</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>2.682</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>2.606</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>2.984</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="D15" s="1" t="n">
+        <v>2.902</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>3.058</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>4.951</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>2.201</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>184</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>175</v>
+      <c r="D19" s="1" t="n">
+        <v>12.667</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="B20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="C20" s="0" t="s">
-        <v>164</v>
+      <c r="B20" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>2.748</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="B21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C21" s="0" t="s">
-        <v>164</v>
+      <c r="B21" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>3.071</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D22" s="0" t="e">
+      <c r="D22" s="1" t="n">
         <f aca="false">AVERAGE(D2:D21)</f>
-        <v>#DIV/0!</v>
+        <v>4.2392</v>
       </c>
     </row>
   </sheetData>
@@ -2335,261 +2529,318 @@
   </sheetPr>
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="18.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="40.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="18.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>207</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <v>3</v>
+      <c r="C2" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>3.265</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>209</v>
+      <c r="D3" s="1" t="n">
+        <v>2.954</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>212</v>
-      </c>
-      <c r="B4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>209</v>
+      <c r="B4" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>3.228</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="B5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>216</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>2.099</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>2.241</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>3.333</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>2.764</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>3.047</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>2.816</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>2.341</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>2.604</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>2.543</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>221</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="D14" s="1" t="n">
+        <v>2.296</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>2.336</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>224</v>
-      </c>
-      <c r="C8" s="0" t="s">
+      <c r="D16" s="1" t="n">
+        <v>2.629</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>2.573</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>2.913</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>2.59</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>3.136</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="C21" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>228</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>230</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>232</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>233</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>234</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>235</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>237</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>238</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>239</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>240</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>241</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>242</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>243</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>245</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>246</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>247</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>248</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>251</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>252</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>224</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>225</v>
+      <c r="D21" s="1" t="n">
+        <v>2.642</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="D22" s="1" t="n">
         <f aca="false">AVERAGE(D2:D21)</f>
-        <v>3</v>
+        <v>2.7175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>